<commit_message>
Update to include trimmed AA sequences (from stop codon)
</commit_message>
<xml_diff>
--- a/pfHRP2_Exon_2_ExPASy.xlsx
+++ b/pfHRP2_Exon_2_ExPASy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kayla\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2D5FF8-ED71-4AF7-836D-B7BFB38AB40F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{44741104-D4FA-407D-927E-6358CB43996B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="72" windowWidth="11988" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11988" windowHeight="12060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pfHRP2_withMeta_ExPASy" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="331">
   <si>
     <t>id</t>
   </si>
@@ -565,9 +565,6 @@
     <t>YSAFNNNLCSKNAKGLNLNKRLLHETQAHVDDAHHAHHVADAHHAHHVADAHHAHHVADAHHAHHAADAHHAADAHHAAAHHATDAHHAAAHHATDAHHAAAHHEAATHCLRH</t>
   </si>
   <si>
-    <t>RCPSCSSCSRCPSCSSCSRCPSCSSCSRCPSCSSCSRCPSCSSCSLCPSCSSCSRCSPCNRCSPCXRCSPCSRCSSCTRCSPCXRCSSRSPCXRCSSRSSCXRCSSRSSCTRCPSCSSCXRCPSCSSCXRCPSCSPCS-CSSRSSCSRCPSCSSCSLCPSCSSCIRRSSCR-CSPCRLCPSRSSCR-CSSCSRCSPCNRCSSCSRCSPC</t>
-  </si>
-  <si>
     <t>DAHHAHHVADAHHAHHVADAHHAHHAADAHHAHHAADAHHAHHAAYAHHAHHAADAHHATDAHHAXDAHHAADAHHAPDAHHAXDAHHAHHAXDAHHAHHAXDAHHAHHAPDAHHAHHAXDAHHAHHAXDAHHAHHAADAHHAHHAADAHHAHHAAYAHHAHHASVAHHADDAHHADYAHHAHHADDAHHAADAHHATDAHHAADAHHA</t>
   </si>
   <si>
@@ -983,6 +980,39 @@
   </si>
   <si>
     <t>TATTCCGCATTTAATAATAACTTGTGTAGCAAAAATGCAAAAGGACTTAATTTAAATAAGAGATTATTACACGAAACTCAAGCACATGTAGATGATGCCCATCATGCTCATCATGTAGCCGATGCCCATCATGCTCATCATGTAGCCGATGCCCATCATGCTCATCATGTAGCCGATGCCCATCTATTCCGCATTTAATAATAACTTGTGTAGCAAAAATGCAAAAGGACTTAATTTAAATAAGAGATTATTACACGAAACTCAAGCACATGTAGCCGATGCCCATCATGCTCATCATGCAGCCGATGCCCATCATGCTCATCATGCAACCGATGCTCTTCATGCAGCCGATGCTCACCATGCAACCGATGCTCACCATGCAGCCGCACACCACCAAGCTGCCACACATTGCCTACGCCATAATGCTCACCATGCAGCTGATGCTCATCACGCTCATCATGCAGCCGATGCTCACCATGCAGCCGATGCTCATCATGCAGCCGCACACCATGCAACTGATGCTCACCATGCAGCCGCACACCATGCAACCGATGCTCACCATGCAGCCGCACACCACGAAGCCGCCACACATTGCCTACGCCATA</t>
+  </si>
+  <si>
+    <t>trimmed_ExPASy_aa_sequence</t>
+  </si>
+  <si>
+    <t>QKEINLNKRLLHETQAHVDDAHHAHHVADAHHAHHVADAHHAHHAADAHHAHHAADAHHAHHAAYAHHAHHASDAHHAADAHHAAYAHHAHHAADAHHAADAHHATDAHHAADAHHATDAHHAHHAADAHHAAAHHATDAHHDAPHHEAPPDCQPHNAAAHHEAATHCLR</t>
+  </si>
+  <si>
+    <t>FPHFNNNLCSKNAKGLNLNKRLLHETQAHVDDAHHAHHVADAHHAHHVADAHHAHHAADAHHAHHAADAHHAHHAAYAHHAHHAADAHHATDAHHAADAHHAADAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHASDAHHAADAHHAAYAHHAHHAADAHHAADAHHATDAHHAADAHHAAAHHATDAHHASAHHKSATH</t>
+  </si>
+  <si>
+    <t>KRLLHETQAHVDDAHHAHHVADAHHAHHAADAHHAAYAHHAHHAADAHHAADAHHATDAHHAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADSPSCSSCSLCPSCSSCIRCSSCIRCSSCS</t>
+  </si>
+  <si>
+    <t>LLHETQAHVDDAHHAHHVADAHHAHHVADAHHAHHVADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHASDAHHADDAHHAADAHHAADAHHAHHAADAHHAADAHHAADAHHAADAHHAVDAHHATDAHHAHHAADAHHAAAHHANDAHHATDAHHAAAHHAR</t>
+  </si>
+  <si>
+    <t>GVGNVWRLRGVRLHGEHRLHGVRLHGEHQLHGVRLHDEHRLHGEHRLHDEHQLHGEHDGHRXXXEYGVGNVWRLRGVRVHGEHRLHGVRLHGEHQLHGVRLHDEHDGHRLHDEHDGHRLHDEHDGHRLHDEHDGHHLHVLEFRVIISYLN</t>
+  </si>
+  <si>
+    <t>LNLNKRLLHETQAQVDDAHHAHHVFRI</t>
+  </si>
+  <si>
+    <t>IYSAFNNNLCSKNAKGLNLNKRLLHETQAHVDDAHHAHHVAYAHHAHHASDAHHAPDAHHAAYAHHAHHAPDAHHAADAHHAPDAHHAPAHHATDAHHEAAHHATDAHHAPAHHEPPTHCLRHTDAHHAAAHHQPATHCLRH</t>
+  </si>
+  <si>
+    <t>YSALNNNLCSKNAKGLNLNKRLLHETQAHVDDAHHAHHVADAHHAHHVADAHHAHHAADAHHAHHAADAHHAHHAAYAHHAHHASDAHHAPDAHHAAYAHHAHHAADAHHAPDAHHAAXAHHATDAHHAADAHHAADAHHAADAHHATDAHHAHHAADAHHAAAHHATDAHHAAAHHATDAHHAAAHHEAATHCLRHXADAHHAADAHHAAAHHATDAHHAAAHHATDAHHAVAHHKAATHCLPH</t>
+  </si>
+  <si>
+    <t>LHETQAHVDDAHHAHHVADAHHAHHVADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHAHHAADAHHATDAHHAAHAHHAADAHHAADAHHAV</t>
+  </si>
+  <si>
+    <t>YSAFNNNLCSKNAKGLNLNKRLLHETQAHVDDAHHAHHVADAHHAHHVADAHHAHHVADAHLFRI</t>
   </si>
 </sst>
 </file>
@@ -1823,10 +1853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1836,9 +1866,10 @@
     <col min="4" max="4" width="13.44140625" customWidth="1"/>
     <col min="5" max="5" width="20.5546875" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1857,8 +1888,11 @@
       <c r="F1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1877,8 +1911,11 @@
       <c r="F2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1897,8 +1934,11 @@
       <c r="F3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1917,8 +1957,11 @@
       <c r="F4" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1937,8 +1980,11 @@
       <c r="F5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1957,8 +2003,11 @@
       <c r="F6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1977,8 +2026,11 @@
       <c r="F7" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1997,8 +2049,11 @@
       <c r="F8" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2017,8 +2072,11 @@
       <c r="F9" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2037,8 +2095,11 @@
       <c r="F10" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2057,8 +2118,11 @@
       <c r="F11" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -2077,8 +2141,11 @@
       <c r="F12" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2097,8 +2164,11 @@
       <c r="F13" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -2117,8 +2187,11 @@
       <c r="F14" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2137,8 +2210,11 @@
       <c r="F15" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2157,8 +2233,11 @@
       <c r="F16" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2177,8 +2256,11 @@
       <c r="F17" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2197,8 +2279,11 @@
       <c r="F18" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -2217,8 +2302,11 @@
       <c r="F19" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -2237,8 +2325,11 @@
       <c r="F20" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -2257,8 +2348,11 @@
       <c r="F21" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2277,8 +2371,11 @@
       <c r="F22" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>50</v>
       </c>
@@ -2297,8 +2394,11 @@
       <c r="F23" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -2317,8 +2417,11 @@
       <c r="F24" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -2337,8 +2440,11 @@
       <c r="F25" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -2357,8 +2463,11 @@
       <c r="F26" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -2377,8 +2486,11 @@
       <c r="F27" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -2397,8 +2509,11 @@
       <c r="F28" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -2417,8 +2532,11 @@
       <c r="F29" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -2437,8 +2555,11 @@
       <c r="F30" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -2457,8 +2578,11 @@
       <c r="F31" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -2477,8 +2601,11 @@
       <c r="F32" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -2497,8 +2624,11 @@
       <c r="F33" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>73</v>
       </c>
@@ -2517,8 +2647,11 @@
       <c r="F34" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -2537,8 +2670,11 @@
       <c r="F35" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>78</v>
       </c>
@@ -2549,16 +2685,19 @@
         <v>181</v>
       </c>
       <c r="D36" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="E36" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="F36" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="G36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -2566,7 +2705,7 @@
         <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D37" t="s">
         <v>153</v>
@@ -2577,8 +2716,11 @@
       <c r="F37" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -2586,7 +2728,7 @@
         <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D38" t="s">
         <v>153</v>
@@ -2597,8 +2739,11 @@
       <c r="F38" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -2606,7 +2751,7 @@
         <v>85</v>
       </c>
       <c r="C39" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D39" t="s">
         <v>162</v>
@@ -2617,8 +2762,11 @@
       <c r="F39" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>86</v>
       </c>
@@ -2626,7 +2774,7 @@
         <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D40" t="s">
         <v>162</v>
@@ -2637,8 +2785,11 @@
       <c r="F40" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2646,7 +2797,7 @@
         <v>89</v>
       </c>
       <c r="C41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D41" t="s">
         <v>153</v>
@@ -2657,8 +2808,11 @@
       <c r="F41" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>90</v>
       </c>
@@ -2677,8 +2831,11 @@
       <c r="F42" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>93</v>
       </c>
@@ -2697,8 +2854,11 @@
       <c r="F43" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>96</v>
       </c>
@@ -2706,7 +2866,7 @@
         <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D44" t="s">
         <v>162</v>
@@ -2717,8 +2877,11 @@
       <c r="F44" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -2726,7 +2889,7 @@
         <v>99</v>
       </c>
       <c r="C45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D45" t="s">
         <v>148</v>
@@ -2737,8 +2900,11 @@
       <c r="F45" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>100</v>
       </c>
@@ -2757,8 +2923,11 @@
       <c r="F46" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -2766,7 +2935,7 @@
         <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D47" t="s">
         <v>148</v>
@@ -2777,8 +2946,11 @@
       <c r="F47" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -2786,7 +2958,7 @@
         <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D48" t="s">
         <v>179</v>
@@ -2797,8 +2969,11 @@
       <c r="F48" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>107</v>
       </c>
@@ -2806,7 +2981,7 @@
         <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D49" t="s">
         <v>148</v>
@@ -2817,8 +2992,11 @@
       <c r="F49" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -2826,7 +3004,7 @@
         <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D50" t="s">
         <v>148</v>
@@ -2837,8 +3015,11 @@
       <c r="F50" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2846,7 +3027,7 @@
         <v>112</v>
       </c>
       <c r="C51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D51" t="s">
         <v>153</v>
@@ -2857,8 +3038,11 @@
       <c r="F51" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>113</v>
       </c>
@@ -2866,7 +3050,7 @@
         <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D52" t="s">
         <v>153</v>
@@ -2877,8 +3061,11 @@
       <c r="F52" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -2886,7 +3073,7 @@
         <v>116</v>
       </c>
       <c r="C53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D53" t="s">
         <v>153</v>
@@ -2897,8 +3084,11 @@
       <c r="F53" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>117</v>
       </c>
@@ -2906,7 +3096,7 @@
         <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D54" t="s">
         <v>162</v>
@@ -2917,8 +3107,11 @@
       <c r="F54" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -2926,7 +3119,7 @@
         <v>120</v>
       </c>
       <c r="C55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D55" t="s">
         <v>153</v>
@@ -2937,8 +3130,11 @@
       <c r="F55" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>121</v>
       </c>
@@ -2946,7 +3142,7 @@
         <v>122</v>
       </c>
       <c r="C56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D56" t="s">
         <v>153</v>
@@ -2957,8 +3153,11 @@
       <c r="F56" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G56" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>123</v>
       </c>
@@ -2966,7 +3165,7 @@
         <v>124</v>
       </c>
       <c r="C57" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D57" t="s">
         <v>162</v>
@@ -2977,8 +3176,11 @@
       <c r="F57" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -2986,7 +3188,7 @@
         <v>126</v>
       </c>
       <c r="C58" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D58" t="s">
         <v>162</v>
@@ -2997,8 +3199,11 @@
       <c r="F58" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>127</v>
       </c>
@@ -3017,8 +3222,11 @@
       <c r="F59" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>130</v>
       </c>
@@ -3026,7 +3234,7 @@
         <v>131</v>
       </c>
       <c r="C60" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D60" t="s">
         <v>148</v>
@@ -3037,8 +3245,11 @@
       <c r="F60" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>132</v>
       </c>
@@ -3046,7 +3257,7 @@
         <v>133</v>
       </c>
       <c r="C61" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D61" t="s">
         <v>148</v>
@@ -3057,8 +3268,11 @@
       <c r="F61" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>134</v>
       </c>
@@ -3066,7 +3280,7 @@
         <v>135</v>
       </c>
       <c r="C62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D62" t="s">
         <v>162</v>
@@ -3077,8 +3291,11 @@
       <c r="F62" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>136</v>
       </c>
@@ -3086,7 +3303,7 @@
         <v>137</v>
       </c>
       <c r="C63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D63" t="s">
         <v>162</v>
@@ -3097,8 +3314,11 @@
       <c r="F63" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>138</v>
       </c>
@@ -3117,8 +3337,11 @@
       <c r="F64" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>141</v>
       </c>
@@ -3126,7 +3349,7 @@
         <v>142</v>
       </c>
       <c r="C65" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D65" t="s">
         <v>153</v>
@@ -3137,8 +3360,11 @@
       <c r="F65" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>143</v>
       </c>
@@ -3146,7 +3372,7 @@
         <v>144</v>
       </c>
       <c r="C66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D66" t="s">
         <v>148</v>
@@ -3157,36 +3383,42 @@
       <c r="F66" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>207</v>
+      </c>
+      <c r="B67" t="s">
+        <v>242</v>
+      </c>
+      <c r="C67" t="s">
+        <v>279</v>
+      </c>
+      <c r="D67" t="s">
+        <v>280</v>
+      </c>
+      <c r="E67" t="s">
+        <v>160</v>
+      </c>
+      <c r="F67" t="s">
+        <v>160</v>
+      </c>
+      <c r="G67" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>208</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>243</v>
       </c>
-      <c r="C67" t="s">
-        <v>280</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="C68" t="s">
         <v>281</v>
-      </c>
-      <c r="E67" t="s">
-        <v>160</v>
-      </c>
-      <c r="F67" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>209</v>
-      </c>
-      <c r="B68" t="s">
-        <v>244</v>
-      </c>
-      <c r="C68" t="s">
-        <v>282</v>
       </c>
       <c r="D68" t="s">
         <v>148</v>
@@ -3197,16 +3429,19 @@
       <c r="F68" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G68" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C69" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D69" t="s">
         <v>148</v>
@@ -3217,16 +3452,19 @@
       <c r="F69" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B70" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C70" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D70" t="s">
         <v>147</v>
@@ -3237,16 +3475,19 @@
       <c r="F70" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G70" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B71" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C71" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D71" t="s">
         <v>147</v>
@@ -3257,16 +3498,19 @@
       <c r="F71" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C72" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D72" t="s">
         <v>153</v>
@@ -3277,16 +3521,19 @@
       <c r="F72" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G72" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B73" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C73" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D73" t="s">
         <v>148</v>
@@ -3297,16 +3544,19 @@
       <c r="F73" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G73" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B74" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C74" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D74" t="s">
         <v>148</v>
@@ -3317,16 +3567,19 @@
       <c r="F74" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G74" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B75" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C75" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D75" t="s">
         <v>148</v>
@@ -3337,16 +3590,19 @@
       <c r="F75" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G75" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B76" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C76" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D76" t="s">
         <v>148</v>
@@ -3357,16 +3613,19 @@
       <c r="F76" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G76" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B77" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C77" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D77" t="s">
         <v>147</v>
@@ -3377,16 +3636,19 @@
       <c r="F77" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G77" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B78" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C78" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D78" t="s">
         <v>148</v>
@@ -3397,16 +3659,19 @@
       <c r="F78" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G78" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B79" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C79" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D79" t="s">
         <v>147</v>
@@ -3417,16 +3682,19 @@
       <c r="F79" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G79" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B80" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C80" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D80" t="s">
         <v>148</v>
@@ -3437,16 +3705,19 @@
       <c r="F80" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G80" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B81" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C81" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D81" t="s">
         <v>147</v>
@@ -3457,16 +3728,19 @@
       <c r="F81" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G81" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C82" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D82" t="s">
         <v>147</v>
@@ -3477,16 +3751,19 @@
       <c r="F82" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B83" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C83" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D83" t="s">
         <v>153</v>
@@ -3497,16 +3774,19 @@
       <c r="F83" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G83" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B84" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C84" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D84" t="s">
         <v>147</v>
@@ -3517,16 +3797,19 @@
       <c r="F84" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G84" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B85" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C85" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D85" t="s">
         <v>148</v>
@@ -3537,16 +3820,19 @@
       <c r="F85" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G85" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C86" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D86" t="s">
         <v>147</v>
@@ -3557,16 +3843,19 @@
       <c r="F86" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G86" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B87" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C87" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D87" t="s">
         <v>148</v>
@@ -3577,16 +3866,19 @@
       <c r="F87" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G87" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B88" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C88" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D88" t="s">
         <v>148</v>
@@ -3597,16 +3889,19 @@
       <c r="F88" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G88" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B89" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C89" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D89" t="s">
         <v>147</v>
@@ -3617,36 +3912,42 @@
       <c r="F89" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G89" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>265</v>
+      </c>
+      <c r="B90" t="s">
         <v>266</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
+        <v>304</v>
+      </c>
+      <c r="D90" t="s">
+        <v>280</v>
+      </c>
+      <c r="E90" t="s">
+        <v>160</v>
+      </c>
+      <c r="F90" t="s">
+        <v>160</v>
+      </c>
+      <c r="G90" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>230</v>
+      </c>
+      <c r="B91" t="s">
         <v>267</v>
       </c>
-      <c r="C90" t="s">
-        <v>305</v>
-      </c>
-      <c r="D90" t="s">
-        <v>281</v>
-      </c>
-      <c r="E90" t="s">
-        <v>160</v>
-      </c>
-      <c r="F90" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>231</v>
-      </c>
-      <c r="B91" t="s">
-        <v>268</v>
-      </c>
       <c r="C91" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D91" t="s">
         <v>153</v>
@@ -3657,16 +3958,19 @@
       <c r="F91" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G91" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B92" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C92" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D92" t="s">
         <v>148</v>
@@ -3677,16 +3981,19 @@
       <c r="F92" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G92" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B93" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C93" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D93" t="s">
         <v>153</v>
@@ -3697,16 +4004,19 @@
       <c r="F93" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G93" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B94" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C94" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D94" t="s">
         <v>179</v>
@@ -3717,16 +4027,19 @@
       <c r="F94" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G94" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B95" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C95" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D95" t="s">
         <v>148</v>
@@ -3737,36 +4050,42 @@
       <c r="F95" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B96" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C96" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D96" t="s">
         <v>147</v>
       </c>
       <c r="E96" t="s">
+        <v>310</v>
+      </c>
+      <c r="F96" t="s">
+        <v>280</v>
+      </c>
+      <c r="G96" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>236</v>
+      </c>
+      <c r="B97" t="s">
+        <v>273</v>
+      </c>
+      <c r="C97" t="s">
         <v>311</v>
-      </c>
-      <c r="F96" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>237</v>
-      </c>
-      <c r="B97" t="s">
-        <v>274</v>
-      </c>
-      <c r="C97" t="s">
-        <v>312</v>
       </c>
       <c r="D97" t="s">
         <v>148</v>
@@ -3777,16 +4096,19 @@
       <c r="F97" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G97" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B98" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C98" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D98" t="s">
         <v>148</v>
@@ -3797,16 +4119,19 @@
       <c r="F98" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G98" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B99" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C99" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D99" t="s">
         <v>148</v>
@@ -3817,16 +4142,19 @@
       <c r="F99" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G99" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B100" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C100" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D100" t="s">
         <v>153</v>
@@ -3837,16 +4165,19 @@
       <c r="F100" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G100" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B101" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C101" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D101" t="s">
         <v>153</v>
@@ -3857,16 +4188,19 @@
       <c r="F101" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G101" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B102" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C102" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D102" t="s">
         <v>148</v>
@@ -3877,16 +4211,19 @@
       <c r="F102" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G102" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>318</v>
+      </c>
+      <c r="B103" t="s">
         <v>319</v>
       </c>
-      <c r="B103" t="s">
-        <v>320</v>
-      </c>
       <c r="C103" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D103" t="s">
         <v>147</v>
@@ -3897,9 +4234,12 @@
       <c r="F103" t="s">
         <v>160</v>
       </c>
+      <c r="G103" t="s">
+        <v>330</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>